<commit_message>
Added colors to drawing sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/auslosungsformular_winzig.xlsx
+++ b/src/main/resources/auslosungsformular_winzig.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suter\Documents\GridCalculator\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="135" windowWidth="20115" windowHeight="9525"/>
   </bookViews>
@@ -226,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -335,21 +340,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -408,39 +398,65 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="double">
-        <color indexed="64"/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color rgb="FF0070C0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="double">
-        <color indexed="64"/>
+      <right style="thick">
+        <color rgb="FF0070C0"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <top style="thick">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF0070C0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -449,7 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,7 +505,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -499,12 +514,74 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -539,88 +616,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -633,6 +655,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -681,7 +706,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -716,7 +741,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -931,7 +956,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C8" sqref="C8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,43 +978,43 @@
         <v>1</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="53"/>
       <c r="I1" s="7"/>
       <c r="J1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="7"/>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="28"/>
+      <c r="M1" s="55"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="9">
-        <v>41938</v>
+        <v>42309</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="39"/>
       <c r="I2" s="10"/>
       <c r="J2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="12"/>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="30"/>
+      <c r="M2" s="57"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1018,173 +1043,174 @@
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="31" t="s">
+      <c r="L4" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="32"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="70" t="s">
+      <c r="M4" s="59"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35" t="s">
+      <c r="B5" s="63"/>
+      <c r="C5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="35" t="s">
+      <c r="D5" s="20"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
       <c r="J5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="K5" s="13"/>
-      <c r="L5" s="33" t="s">
+      <c r="L5" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="34"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="22" t="s">
+      <c r="M5" s="61"/>
+    </row>
+    <row r="6" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="71"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="15" t="s">
+      <c r="F6" s="68"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="22" t="s">
+    <row r="7" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="71"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="62"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="15" t="s">
+      <c r="F7" s="68"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="66" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="65"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="23" t="s">
+    <row r="8" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="65"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="21" t="s">
+      <c r="F8" s="68"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="67" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D9" s="16"/>
+    <row r="9" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="15"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
-      <c r="F14" s="18" t="s">
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
+      <c r="F14" s="17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="54"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="59"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
       <c r="F15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="55"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="47"/>
       <c r="F16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
       <c r="F17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
     </row>
     <row r="19" spans="2:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B19" s="38"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
-      <c r="F19" s="18" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="F19" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="46"/>
-      <c r="F20" s="19" t="s">
+      <c r="C20" s="31"/>
+      <c r="D20" s="32"/>
+      <c r="F20" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="48"/>
-      <c r="F21" s="19" t="s">
+      <c r="B21" s="23"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="34"/>
+      <c r="F21" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="38"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:D19"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="F5:I5"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="C20:D22"/>
     <mergeCell ref="F2:H2"/>
@@ -1199,12 +1225,11 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:D19"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="74" orientation="landscape" r:id="rId1"/>

</xml_diff>